<commit_message>
update test case for testing design technique
</commit_message>
<xml_diff>
--- a/Rookies_QCHN_5. Test Design Technique/Đặng Ngọc Điệp_Rookies QC B6_Test design Technique homework.xlsx
+++ b/Rookies_QCHN_5. Test Design Technique/Đặng Ngọc Điệp_Rookies QC B6_Test design Technique homework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dangdiep/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B260E358-34F4-134E-8CDE-47D29C31B353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC1994E-4EE9-5741-9C03-6CAFF3824CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1820" yWindow="1480" windowWidth="19160" windowHeight="14420" tabRatio="840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,7 +933,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="479">
   <si>
     <r>
       <t xml:space="preserve">Security Classification: </t>
@@ -2689,15 +2689,6 @@
     <t>Verify that the discounted price will show three commas with a value is 1000000000</t>
   </si>
   <si>
-    <t>Verify that the discounted price will be rounded up if the decimal fraction is 0.6</t>
-  </si>
-  <si>
-    <t>Verify that the discounted price will be rounded up if the decimal fraction is 0.5</t>
-  </si>
-  <si>
-    <t>Verify that the discounted price will be rounded down if the decimal fraction is 0.4</t>
-  </si>
-  <si>
     <t>2. Write test design for View Product function – Display photos</t>
   </si>
   <si>
@@ -2735,6 +2726,96 @@
   </si>
   <si>
     <t>Verify that the "&gt;" button is enabled when it is before the last photo of the photo list</t>
+  </si>
+  <si>
+    <t>The original price does not show comma</t>
+  </si>
+  <si>
+    <t>The original price show one comma</t>
+  </si>
+  <si>
+    <t>The original price show two commas</t>
+  </si>
+  <si>
+    <t>The original price show three commas</t>
+  </si>
+  <si>
+    <t>Verify that the discounted price will be rounded up to the nearest integer if the decimal fraction is 0.6</t>
+  </si>
+  <si>
+    <t>Verify that the discounted price will be rounded up to the nearest integer if the decimal fraction is 0.5</t>
+  </si>
+  <si>
+    <t>Verify that the discounted price will be rounded down to the nearest integer if the decimal fraction is 0.4</t>
+  </si>
+  <si>
+    <t>13000.06</t>
+  </si>
+  <si>
+    <t>13000.05</t>
+  </si>
+  <si>
+    <t>13000.04</t>
+  </si>
+  <si>
+    <t>- Select product
+- Click on it</t>
+  </si>
+  <si>
+    <t>User account should be present in application</t>
+  </si>
+  <si>
+    <t>- There is 1 photo display on the photo list
+- The big photo frame display that photo
+- Both "&lt;" button and "&gt;" button are disabled</t>
+  </si>
+  <si>
+    <t>- There are 4 photos display on the photo list
+- The big photo frame display the first photo of photo list</t>
+  </si>
+  <si>
+    <t>- There are 5 photos display on the photo list
+- The big photo frame display the first photo of photo list</t>
+  </si>
+  <si>
+    <t>- The discounted price is rounded up to the nearest integer
+- The discounted price use comma as decimal separator to separate groups of thousands, millions, etc</t>
+  </si>
+  <si>
+    <t>- The discounted price is rounded down to the nearest integer
+- The discounted price use comma as decimal separator to separate groups of thousands, millions, etc</t>
+  </si>
+  <si>
+    <t>The first photo of the photo list is displayed on the big photo frame</t>
+  </si>
+  <si>
+    <t>Both "&lt;" button and "&gt;" button are disabled</t>
+  </si>
+  <si>
+    <t>The "&lt;" button is disabled</t>
+  </si>
+  <si>
+    <t>The "&gt;" button is disabled</t>
+  </si>
+  <si>
+    <t>The "&lt;" button is enabled</t>
+  </si>
+  <si>
+    <t>The "&gt;" button is enabled</t>
+  </si>
+  <si>
+    <t>Both "&lt;" button and "&gt;" button are enabled</t>
+  </si>
+  <si>
+    <t>No photo display on the photo list and the big photo frame (or the big photo frame display the default image)</t>
+  </si>
+  <si>
+    <t>1. Go to the Admin page
+2. Enter the value of original price</t>
+  </si>
+  <si>
+    <t>1. Go to the Admin page
+2. Enter the value of discounted price</t>
   </si>
 </sst>
 </file>
@@ -3736,7 +3817,7 @@
     <xf numFmtId="166" fontId="56" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="57" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -4387,9 +4468,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -4400,10 +4478,10 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="18" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6198,8 +6276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13"/>
@@ -6472,9 +6550,15 @@
       <c r="B20" s="52" t="s">
         <v>420</v>
       </c>
-      <c r="C20" s="52"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="54"/>
+      <c r="C20" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>452</v>
+      </c>
+      <c r="E20" s="54">
+        <v>998</v>
+      </c>
       <c r="F20" s="52"/>
       <c r="G20" s="52"/>
       <c r="H20" s="52"/>
@@ -6488,9 +6572,15 @@
       <c r="B21" s="52" t="s">
         <v>421</v>
       </c>
-      <c r="C21" s="52"/>
-      <c r="D21" s="59"/>
-      <c r="E21" s="54"/>
+      <c r="C21" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D21" s="53" t="s">
+        <v>452</v>
+      </c>
+      <c r="E21" s="54">
+        <v>999</v>
+      </c>
       <c r="F21" s="52"/>
       <c r="G21" s="52"/>
       <c r="H21" s="52"/>
@@ -6504,9 +6594,15 @@
       <c r="B22" s="52" t="s">
         <v>422</v>
       </c>
-      <c r="C22" s="52"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="54"/>
+      <c r="C22" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="E22" s="54">
+        <v>1000</v>
+      </c>
       <c r="F22" s="52"/>
       <c r="G22" s="52"/>
       <c r="H22" s="52"/>
@@ -6520,9 +6616,15 @@
       <c r="B23" s="52" t="s">
         <v>423</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="54"/>
-      <c r="E23" s="54"/>
+      <c r="C23" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D23" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="E23" s="54">
+        <v>999998</v>
+      </c>
       <c r="F23" s="52"/>
       <c r="G23" s="52"/>
       <c r="H23" s="52"/>
@@ -6536,9 +6638,15 @@
       <c r="B24" s="52" t="s">
         <v>424</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="54"/>
-      <c r="E24" s="54"/>
+      <c r="C24" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D24" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="E24" s="54">
+        <v>999999</v>
+      </c>
       <c r="F24" s="52"/>
       <c r="G24" s="52"/>
       <c r="H24" s="52"/>
@@ -6552,9 +6660,15 @@
       <c r="B25" s="52" t="s">
         <v>425</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="54"/>
+      <c r="C25" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>454</v>
+      </c>
+      <c r="E25" s="54">
+        <v>1000000</v>
+      </c>
       <c r="F25" s="52"/>
       <c r="G25" s="52"/>
       <c r="H25" s="52"/>
@@ -6568,9 +6682,15 @@
       <c r="B26" s="52" t="s">
         <v>426</v>
       </c>
-      <c r="C26" s="52"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
+      <c r="C26" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>454</v>
+      </c>
+      <c r="E26" s="54">
+        <v>999999998</v>
+      </c>
       <c r="F26" s="52"/>
       <c r="G26" s="52"/>
       <c r="H26" s="52"/>
@@ -6584,9 +6704,15 @@
       <c r="B27" s="52" t="s">
         <v>427</v>
       </c>
-      <c r="C27" s="52"/>
-      <c r="D27" s="54"/>
-      <c r="E27" s="54"/>
+      <c r="C27" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D27" s="53" t="s">
+        <v>454</v>
+      </c>
+      <c r="E27" s="54">
+        <v>999999999</v>
+      </c>
       <c r="F27" s="52"/>
       <c r="G27" s="52"/>
       <c r="H27" s="52"/>
@@ -6600,9 +6726,15 @@
       <c r="B28" s="52" t="s">
         <v>428</v>
       </c>
-      <c r="C28" s="52"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
+      <c r="C28" s="52" t="s">
+        <v>477</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>455</v>
+      </c>
+      <c r="E28" s="54">
+        <v>1000000000</v>
+      </c>
       <c r="F28" s="52"/>
       <c r="G28" s="52"/>
       <c r="H28" s="52"/>
@@ -6628,9 +6760,15 @@
       <c r="B30" s="52" t="s">
         <v>430</v>
       </c>
-      <c r="C30" s="52"/>
-      <c r="D30" s="53"/>
-      <c r="E30" s="54"/>
+      <c r="C30" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>452</v>
+      </c>
+      <c r="E30" s="54">
+        <v>998</v>
+      </c>
       <c r="F30" s="52"/>
       <c r="G30" s="52"/>
       <c r="H30" s="52"/>
@@ -6644,9 +6782,15 @@
       <c r="B31" s="52" t="s">
         <v>431</v>
       </c>
-      <c r="C31" s="52"/>
-      <c r="D31" s="59"/>
-      <c r="E31" s="54"/>
+      <c r="C31" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D31" s="53" t="s">
+        <v>452</v>
+      </c>
+      <c r="E31" s="54">
+        <v>999</v>
+      </c>
       <c r="F31" s="52"/>
       <c r="G31" s="52"/>
       <c r="H31" s="52"/>
@@ -6660,9 +6804,15 @@
       <c r="B32" s="52" t="s">
         <v>432</v>
       </c>
-      <c r="C32" s="52"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="54"/>
+      <c r="C32" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="E32" s="54">
+        <v>1000</v>
+      </c>
       <c r="F32" s="52"/>
       <c r="G32" s="52"/>
       <c r="H32" s="52"/>
@@ -6676,9 +6826,15 @@
       <c r="B33" s="52" t="s">
         <v>433</v>
       </c>
-      <c r="C33" s="52"/>
-      <c r="D33" s="54"/>
-      <c r="E33" s="54"/>
+      <c r="C33" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D33" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="E33" s="54">
+        <v>999998</v>
+      </c>
       <c r="F33" s="52"/>
       <c r="G33" s="52"/>
       <c r="H33" s="52"/>
@@ -6692,9 +6848,15 @@
       <c r="B34" s="52" t="s">
         <v>434</v>
       </c>
-      <c r="C34" s="52"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
+      <c r="C34" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D34" s="53" t="s">
+        <v>453</v>
+      </c>
+      <c r="E34" s="54">
+        <v>999999</v>
+      </c>
       <c r="F34" s="52"/>
       <c r="G34" s="52"/>
       <c r="H34" s="52"/>
@@ -6708,9 +6870,15 @@
       <c r="B35" s="52" t="s">
         <v>435</v>
       </c>
-      <c r="C35" s="52"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="54"/>
+      <c r="C35" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D35" s="53" t="s">
+        <v>454</v>
+      </c>
+      <c r="E35" s="54">
+        <v>1000000</v>
+      </c>
       <c r="F35" s="52"/>
       <c r="G35" s="52"/>
       <c r="H35" s="52"/>
@@ -6724,9 +6892,15 @@
       <c r="B36" s="52" t="s">
         <v>436</v>
       </c>
-      <c r="C36" s="52"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
+      <c r="C36" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D36" s="53" t="s">
+        <v>454</v>
+      </c>
+      <c r="E36" s="54">
+        <v>999999998</v>
+      </c>
       <c r="F36" s="52"/>
       <c r="G36" s="52"/>
       <c r="H36" s="52"/>
@@ -6740,9 +6914,15 @@
       <c r="B37" s="52" t="s">
         <v>437</v>
       </c>
-      <c r="C37" s="52"/>
-      <c r="D37" s="54"/>
-      <c r="E37" s="54"/>
+      <c r="C37" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D37" s="53" t="s">
+        <v>454</v>
+      </c>
+      <c r="E37" s="54">
+        <v>999999999</v>
+      </c>
       <c r="F37" s="52"/>
       <c r="G37" s="52"/>
       <c r="H37" s="52"/>
@@ -6756,57 +6936,81 @@
       <c r="B38" s="52" t="s">
         <v>438</v>
       </c>
-      <c r="C38" s="52"/>
-      <c r="D38" s="54"/>
-      <c r="E38" s="54"/>
+      <c r="C38" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D38" s="53" t="s">
+        <v>455</v>
+      </c>
+      <c r="E38" s="54">
+        <v>1000000000</v>
+      </c>
       <c r="F38" s="52"/>
       <c r="G38" s="52"/>
       <c r="H38" s="52"/>
       <c r="I38" s="61"/>
     </row>
-    <row r="39" spans="1:9" s="48" customFormat="1" ht="28">
+    <row r="39" spans="1:9" s="48" customFormat="1" ht="70">
       <c r="A39" s="62">
         <f t="shared" ref="A39:A41" ca="1" si="1">IF(OFFSET(A39,-1,0) ="",OFFSET(A39,-2,0)+1,OFFSET(A39,-1,0)+1 )</f>
         <v>10</v>
       </c>
       <c r="B39" s="52" t="s">
-        <v>439</v>
-      </c>
-      <c r="C39" s="52"/>
-      <c r="D39" s="54"/>
-      <c r="E39" s="54"/>
+        <v>456</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D39" s="54" t="s">
+        <v>467</v>
+      </c>
+      <c r="E39" s="54" t="s">
+        <v>459</v>
+      </c>
       <c r="F39" s="52"/>
       <c r="G39" s="52"/>
       <c r="H39" s="52"/>
       <c r="I39" s="62"/>
     </row>
-    <row r="40" spans="1:9" s="48" customFormat="1" ht="28">
+    <row r="40" spans="1:9" s="48" customFormat="1" ht="70">
       <c r="A40" s="62">
         <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="B40" s="52" t="s">
-        <v>440</v>
-      </c>
-      <c r="C40" s="52"/>
-      <c r="D40" s="54"/>
-      <c r="E40" s="54"/>
+        <v>457</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D40" s="54" t="s">
+        <v>467</v>
+      </c>
+      <c r="E40" s="54" t="s">
+        <v>460</v>
+      </c>
       <c r="F40" s="52"/>
       <c r="G40" s="52"/>
       <c r="H40" s="52"/>
       <c r="I40" s="62"/>
     </row>
-    <row r="41" spans="1:9" s="48" customFormat="1" ht="28">
+    <row r="41" spans="1:9" s="48" customFormat="1" ht="70">
       <c r="A41" s="62">
         <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
       <c r="B41" s="52" t="s">
-        <v>441</v>
-      </c>
-      <c r="C41" s="52"/>
-      <c r="D41" s="54"/>
-      <c r="E41" s="60"/>
+        <v>458</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>478</v>
+      </c>
+      <c r="D41" s="54" t="s">
+        <v>468</v>
+      </c>
+      <c r="E41" s="60" t="s">
+        <v>461</v>
+      </c>
       <c r="F41" s="52"/>
       <c r="G41" s="52"/>
       <c r="H41" s="52"/>
@@ -6815,7 +7019,7 @@
     <row r="42" spans="1:9" s="48" customFormat="1" ht="14">
       <c r="A42" s="67"/>
       <c r="B42" s="193" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C42" s="194"/>
       <c r="D42" s="195"/>
@@ -6825,84 +7029,114 @@
       <c r="H42" s="66"/>
       <c r="I42" s="69"/>
     </row>
-    <row r="43" spans="1:9" s="48" customFormat="1" ht="28">
+    <row r="43" spans="1:9" s="48" customFormat="1" ht="42">
       <c r="A43" s="52">
         <v>1</v>
       </c>
       <c r="B43" s="52" t="s">
-        <v>443</v>
-      </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="54"/>
+        <v>440</v>
+      </c>
+      <c r="C43" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D43" s="237" t="s">
+        <v>476</v>
+      </c>
+      <c r="E43" s="54" t="s">
+        <v>463</v>
+      </c>
       <c r="F43" s="52"/>
       <c r="G43" s="52"/>
       <c r="H43" s="52"/>
       <c r="I43" s="62"/>
     </row>
-    <row r="44" spans="1:9" s="48" customFormat="1" ht="29" customHeight="1">
+    <row r="44" spans="1:9" s="48" customFormat="1" ht="56">
       <c r="A44" s="58">
         <f ca="1">IF(OFFSET(A44,-1,0) ="",OFFSET(A44,-2,0)+1,OFFSET(A44,-1,0)+1 )</f>
         <v>2</v>
       </c>
       <c r="B44" s="52" t="s">
-        <v>444</v>
-      </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="59"/>
-      <c r="E44" s="54"/>
+        <v>441</v>
+      </c>
+      <c r="C44" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D44" s="53" t="s">
+        <v>464</v>
+      </c>
+      <c r="E44" s="54" t="s">
+        <v>463</v>
+      </c>
       <c r="F44" s="52"/>
       <c r="G44" s="52"/>
       <c r="H44" s="52"/>
       <c r="I44" s="62"/>
     </row>
-    <row r="45" spans="1:9" s="48" customFormat="1" ht="28">
+    <row r="45" spans="1:9" s="48" customFormat="1" ht="56">
       <c r="A45" s="58">
         <f ca="1">IF(OFFSET(A45,-1,0) ="",OFFSET(A45,-2,0)+1,OFFSET(A45,-1,0)+1 )</f>
         <v>3</v>
       </c>
       <c r="B45" s="52" t="s">
-        <v>445</v>
-      </c>
-      <c r="C45" s="52"/>
-      <c r="D45" s="60"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="233"/>
-      <c r="G45" s="233"/>
-      <c r="H45" s="233"/>
-      <c r="I45" s="234"/>
-    </row>
-    <row r="46" spans="1:9" s="48" customFormat="1" ht="28">
+        <v>442</v>
+      </c>
+      <c r="C45" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D45" s="53" t="s">
+        <v>465</v>
+      </c>
+      <c r="E45" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F45" s="232"/>
+      <c r="G45" s="232"/>
+      <c r="H45" s="232"/>
+      <c r="I45" s="233"/>
+    </row>
+    <row r="46" spans="1:9" s="48" customFormat="1" ht="56">
       <c r="A46" s="58">
         <f ca="1">IF(OFFSET(A46,-1,0) ="",OFFSET(A46,-2,0)+1,OFFSET(A46,-1,0)+1 )</f>
         <v>4</v>
       </c>
       <c r="B46" s="52" t="s">
-        <v>446</v>
-      </c>
-      <c r="C46" s="52"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="235"/>
-      <c r="G46" s="235"/>
-      <c r="H46" s="235"/>
-      <c r="I46" s="236"/>
-    </row>
-    <row r="47" spans="1:9" s="48" customFormat="1" ht="28">
+        <v>443</v>
+      </c>
+      <c r="C46" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D46" s="53" t="s">
+        <v>466</v>
+      </c>
+      <c r="E46" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F46" s="234"/>
+      <c r="G46" s="234"/>
+      <c r="H46" s="234"/>
+      <c r="I46" s="235"/>
+    </row>
+    <row r="47" spans="1:9" s="48" customFormat="1" ht="56">
       <c r="A47" s="58">
         <f ca="1">IF(OFFSET(A47,-1,0) ="",OFFSET(A47,-2,0)+1,OFFSET(A47,-1,0)+1 )</f>
         <v>5</v>
       </c>
       <c r="B47" s="52" t="s">
-        <v>447</v>
-      </c>
-      <c r="C47" s="52"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="233"/>
-      <c r="G47" s="233"/>
-      <c r="H47" s="233"/>
-      <c r="I47" s="234"/>
+        <v>444</v>
+      </c>
+      <c r="C47" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D47" s="53" t="s">
+        <v>466</v>
+      </c>
+      <c r="E47" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F47" s="232"/>
+      <c r="G47" s="232"/>
+      <c r="H47" s="232"/>
+      <c r="I47" s="233"/>
     </row>
     <row r="48" spans="1:9" s="48" customFormat="1" ht="56">
       <c r="A48" s="58">
@@ -6910,31 +7144,43 @@
         <v>6</v>
       </c>
       <c r="B48" s="52" t="s">
-        <v>448</v>
-      </c>
-      <c r="C48" s="52"/>
-      <c r="D48" s="60"/>
-      <c r="E48" s="54"/>
-      <c r="F48" s="233"/>
-      <c r="G48" s="233"/>
-      <c r="H48" s="233"/>
-      <c r="I48" s="234"/>
+        <v>445</v>
+      </c>
+      <c r="C48" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D48" s="60" t="s">
+        <v>469</v>
+      </c>
+      <c r="E48" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F48" s="232"/>
+      <c r="G48" s="232"/>
+      <c r="H48" s="232"/>
+      <c r="I48" s="233"/>
     </row>
     <row r="49" spans="1:9" s="48" customFormat="1" ht="42">
       <c r="A49" s="58">
         <f t="shared" ref="A49:A54" ca="1" si="2">IF(OFFSET(A49,-1,0) ="",OFFSET(A49,-2,0)+1,OFFSET(A49,-1,0)+1 )</f>
         <v>7</v>
       </c>
-      <c r="B49" s="233" t="s">
-        <v>449</v>
-      </c>
-      <c r="C49" s="52"/>
-      <c r="D49" s="54"/>
-      <c r="E49" s="54"/>
-      <c r="F49" s="233"/>
-      <c r="G49" s="233"/>
-      <c r="H49" s="233"/>
-      <c r="I49" s="234"/>
+      <c r="B49" s="232" t="s">
+        <v>446</v>
+      </c>
+      <c r="C49" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D49" s="54" t="s">
+        <v>470</v>
+      </c>
+      <c r="E49" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F49" s="232"/>
+      <c r="G49" s="232"/>
+      <c r="H49" s="232"/>
+      <c r="I49" s="233"/>
     </row>
     <row r="50" spans="1:9" s="48" customFormat="1" ht="28">
       <c r="A50" s="58">
@@ -6942,15 +7188,21 @@
         <v>8</v>
       </c>
       <c r="B50" s="52" t="s">
-        <v>451</v>
-      </c>
-      <c r="C50" s="52"/>
-      <c r="D50" s="54"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="235"/>
-      <c r="G50" s="235"/>
-      <c r="H50" s="235"/>
-      <c r="I50" s="236"/>
+        <v>448</v>
+      </c>
+      <c r="C50" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D50" s="54" t="s">
+        <v>471</v>
+      </c>
+      <c r="E50" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F50" s="234"/>
+      <c r="G50" s="234"/>
+      <c r="H50" s="234"/>
+      <c r="I50" s="235"/>
     </row>
     <row r="51" spans="1:9" s="48" customFormat="1" ht="28">
       <c r="A51" s="58">
@@ -6958,15 +7210,21 @@
         <v>9</v>
       </c>
       <c r="B51" s="52" t="s">
-        <v>453</v>
-      </c>
-      <c r="C51" s="237"/>
-      <c r="D51" s="238"/>
-      <c r="E51" s="54"/>
-      <c r="F51" s="235"/>
-      <c r="G51" s="235"/>
-      <c r="H51" s="235"/>
-      <c r="I51" s="236"/>
+        <v>450</v>
+      </c>
+      <c r="C51" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D51" s="54" t="s">
+        <v>473</v>
+      </c>
+      <c r="E51" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F51" s="234"/>
+      <c r="G51" s="234"/>
+      <c r="H51" s="234"/>
+      <c r="I51" s="235"/>
     </row>
     <row r="52" spans="1:9" s="48" customFormat="1" ht="28">
       <c r="A52" s="58">
@@ -6974,15 +7232,21 @@
         <v>10</v>
       </c>
       <c r="B52" s="231" t="s">
-        <v>452</v>
-      </c>
-      <c r="C52" s="52"/>
-      <c r="D52" s="60"/>
-      <c r="E52" s="232"/>
-      <c r="F52" s="233"/>
-      <c r="G52" s="233"/>
-      <c r="H52" s="233"/>
-      <c r="I52" s="234"/>
+        <v>449</v>
+      </c>
+      <c r="C52" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D52" s="54" t="s">
+        <v>472</v>
+      </c>
+      <c r="E52" s="54" t="s">
+        <v>463</v>
+      </c>
+      <c r="F52" s="232"/>
+      <c r="G52" s="232"/>
+      <c r="H52" s="232"/>
+      <c r="I52" s="233"/>
     </row>
     <row r="53" spans="1:9" s="48" customFormat="1" ht="28">
       <c r="A53" s="58">
@@ -6990,11 +7254,17 @@
         <v>11</v>
       </c>
       <c r="B53" s="231" t="s">
-        <v>454</v>
-      </c>
-      <c r="C53" s="52"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="232"/>
+        <v>451</v>
+      </c>
+      <c r="C53" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D53" s="54" t="s">
+        <v>474</v>
+      </c>
+      <c r="E53" s="54" t="s">
+        <v>463</v>
+      </c>
       <c r="F53" s="52"/>
       <c r="G53" s="52"/>
       <c r="H53" s="52"/>
@@ -7006,11 +7276,17 @@
         <v>12</v>
       </c>
       <c r="B54" s="231" t="s">
-        <v>450</v>
-      </c>
-      <c r="C54" s="52"/>
-      <c r="D54" s="60"/>
-      <c r="E54" s="232"/>
+        <v>447</v>
+      </c>
+      <c r="C54" s="236" t="s">
+        <v>462</v>
+      </c>
+      <c r="D54" s="54" t="s">
+        <v>475</v>
+      </c>
+      <c r="E54" s="54" t="s">
+        <v>463</v>
+      </c>
       <c r="F54" s="52"/>
       <c r="G54" s="52"/>
       <c r="H54" s="52"/>

</xml_diff>